<commit_message>
survivor - nove data, nove grafy
</commit_message>
<xml_diff>
--- a/survivor_2023_data.xlsx
+++ b/survivor_2023_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tina\Documents\GitHub\personal_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175D27C0-7A4F-4E11-9257-D759A2580F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215A4F65-02B8-47F2-8BFE-0BCC49D66091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="1140" windowWidth="28710" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="255" yWindow="1755" windowWidth="28545" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="event_log" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="130">
   <si>
     <t>DAY</t>
   </si>
@@ -270,9 +270,6 @@
     <t>Tomáš, Žaneta, Jiří, Matěj, Johanka, Adam, Martin, Lída, Barbora, Kristián</t>
   </si>
   <si>
-    <t>Bedna so zeleninou + koreniny</t>
-  </si>
-  <si>
     <t>31:20</t>
   </si>
   <si>
@@ -306,13 +303,130 @@
     <t>1:16:44</t>
   </si>
   <si>
-    <t>2 brambory pre každého</t>
-  </si>
-  <si>
     <t>Slepice, kohout + vejce</t>
   </si>
   <si>
     <t>Sandwich, chipsy, cola</t>
+  </si>
+  <si>
+    <t>2 brambory</t>
+  </si>
+  <si>
+    <t>Zelenina, koreniny</t>
+  </si>
+  <si>
+    <t>6:40</t>
+  </si>
+  <si>
+    <t>Kafe, dort, dopisy</t>
+  </si>
+  <si>
+    <t>Pepa, Andrea, Kateřina, Pítr, Karolína, Filip, Švanci, Pavlína, Kulhy</t>
+  </si>
+  <si>
+    <t>45:28</t>
+  </si>
+  <si>
+    <t>Aukce</t>
+  </si>
+  <si>
+    <t>10:55</t>
+  </si>
+  <si>
+    <t>23:50</t>
+  </si>
+  <si>
+    <t>55:38</t>
+  </si>
+  <si>
+    <t>1:17:54</t>
+  </si>
+  <si>
+    <t>8:51</t>
+  </si>
+  <si>
+    <t>Lednice plná jídla</t>
+  </si>
+  <si>
+    <t>2:0</t>
+  </si>
+  <si>
+    <t>Tomáš, Žaneta, Jiří, Matěj, Johanka, Adam, Martin, Barbora, Kristián</t>
+  </si>
+  <si>
+    <t>46:16</t>
+  </si>
+  <si>
+    <t>Hot-Dog, cola, dopisy</t>
+  </si>
+  <si>
+    <t>1:10:30</t>
+  </si>
+  <si>
+    <t>Výhoda</t>
+  </si>
+  <si>
+    <t>Zisk odměny navíc</t>
+  </si>
+  <si>
+    <t>10:42</t>
+  </si>
+  <si>
+    <t>Výměna členů</t>
+  </si>
+  <si>
+    <t>28:52</t>
+  </si>
+  <si>
+    <t>Pepa, Andrea, Kateřina, Pítr, Karolína, Filip, Švanci, Pavlína, Matěj</t>
+  </si>
+  <si>
+    <t>Tomáš, Žaneta, Jiří, Johanka, Kulhy, Adam, Martin, Barbora, Kristián</t>
+  </si>
+  <si>
+    <t>42:35</t>
+  </si>
+  <si>
+    <t>1:11:54</t>
+  </si>
+  <si>
+    <t>1:19:41</t>
+  </si>
+  <si>
+    <t>1:36:54</t>
+  </si>
+  <si>
+    <t>Pepa, Andrea, Pítr, Karolína, Filip, Tomáš, Pavlína, Matěj</t>
+  </si>
+  <si>
+    <t>Švanci, Žaneta, Jiří, Johanka, Kulhy, Adam, Martin, Barbora, Kristián</t>
+  </si>
+  <si>
+    <t>15:33</t>
+  </si>
+  <si>
+    <t>Jídlo od maminky</t>
+  </si>
+  <si>
+    <t>58:47</t>
+  </si>
+  <si>
+    <t>Empanada, drink, vzkaz</t>
+  </si>
+  <si>
+    <t>6:37</t>
+  </si>
+  <si>
+    <t>19:02</t>
+  </si>
+  <si>
+    <t>50:17</t>
+  </si>
+  <si>
+    <t>50:40</t>
+  </si>
+  <si>
+    <t>1:17:43</t>
   </si>
 </sst>
 </file>
@@ -666,11 +780,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I105"/>
+  <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -753,7 +865,7 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
@@ -874,7 +986,7 @@
         <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F8" t="s">
         <v>16</v>
@@ -1083,7 +1195,7 @@
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
@@ -1207,7 +1319,7 @@
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="F21" t="s">
         <v>12</v>
@@ -1230,10 +1342,10 @@
         <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" t="s">
         <v>78</v>
-      </c>
-      <c r="D22" t="s">
-        <v>79</v>
       </c>
       <c r="F22" t="s">
         <v>16</v>
@@ -1251,13 +1363,13 @@
         <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F23" t="s">
         <v>12</v>
@@ -1266,10 +1378,10 @@
         <v>76</v>
       </c>
       <c r="H23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1280,7 +1392,7 @@
         <v>8</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D24" t="s">
         <v>20</v>
@@ -1292,10 +1404,10 @@
         <v>76</v>
       </c>
       <c r="H24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1306,7 +1418,7 @@
         <v>8</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D25" t="s">
         <v>22</v>
@@ -1327,7 +1439,7 @@
         <v>8</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D26" t="s">
         <v>44</v>
@@ -1351,7 +1463,7 @@
         <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D27" t="s">
         <v>47</v>
@@ -1368,171 +1480,664 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C28" s="1"/>
-      <c r="I28" s="1"/>
+      <c r="A28">
+        <v>21</v>
+      </c>
+      <c r="B28">
+        <v>9</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>93</v>
+      </c>
+      <c r="F28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" t="s">
+        <v>94</v>
+      </c>
+      <c r="H28" t="s">
+        <v>76</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C29" s="1"/>
-      <c r="I29" s="1"/>
+      <c r="A29">
+        <v>23</v>
+      </c>
+      <c r="B29">
+        <v>9</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" t="s">
+        <v>76</v>
+      </c>
+      <c r="H29" t="s">
+        <v>94</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C30" s="1"/>
-      <c r="I30" s="1"/>
+      <c r="A30">
+        <v>24</v>
+      </c>
+      <c r="B30">
+        <v>10</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H30" t="s">
+        <v>76</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C31" s="1"/>
+      <c r="A31">
+        <v>24</v>
+      </c>
+      <c r="B31">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" t="s">
+        <v>30</v>
+      </c>
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C32" s="1"/>
+      <c r="A32">
+        <v>26</v>
+      </c>
+      <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" t="s">
+        <v>52</v>
+      </c>
+      <c r="H32" t="s">
+        <v>33</v>
+      </c>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C33" s="1"/>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>26</v>
+      </c>
+      <c r="B33">
+        <v>10</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" t="s">
+        <v>52</v>
+      </c>
+      <c r="H33" t="s">
+        <v>33</v>
+      </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C34" s="1"/>
-      <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C35" s="1"/>
-      <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C36" s="1"/>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>27</v>
+      </c>
+      <c r="B34">
+        <v>11</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" t="s">
+        <v>102</v>
+      </c>
+      <c r="F34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" t="s">
+        <v>104</v>
+      </c>
+      <c r="H34" t="s">
+        <v>94</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>28</v>
+      </c>
+      <c r="B35">
+        <v>11</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" t="s">
+        <v>106</v>
+      </c>
+      <c r="F35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" t="s">
+        <v>104</v>
+      </c>
+      <c r="H35" t="s">
+        <v>94</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>28</v>
+      </c>
+      <c r="B36">
+        <v>11</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36" t="s">
+        <v>109</v>
+      </c>
+      <c r="F36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" t="s">
+        <v>34</v>
+      </c>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C43" s="1"/>
-    </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C44" s="1"/>
-    </row>
-    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C47" s="1"/>
-    </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C48" s="1"/>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C49" s="1"/>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>30</v>
+      </c>
+      <c r="B37">
+        <v>12</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" t="s">
+        <v>111</v>
+      </c>
+      <c r="F37" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" t="s">
+        <v>51</v>
+      </c>
+      <c r="H37" t="s">
+        <v>28</v>
+      </c>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>31</v>
+      </c>
+      <c r="B38">
+        <v>12</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" t="s">
+        <v>114</v>
+      </c>
+      <c r="H38" t="s">
+        <v>113</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>31</v>
+      </c>
+      <c r="B39">
+        <v>12</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D39" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" t="s">
+        <v>41</v>
+      </c>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>32</v>
+      </c>
+      <c r="B40">
+        <v>12</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D40" t="s">
+        <v>111</v>
+      </c>
+      <c r="F40" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" t="s">
+        <v>43</v>
+      </c>
+      <c r="H40" t="s">
+        <v>24</v>
+      </c>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>32</v>
+      </c>
+      <c r="B41">
+        <v>12</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D41" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" t="s">
+        <v>38</v>
+      </c>
+      <c r="H41" t="s">
+        <v>37</v>
+      </c>
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>32</v>
+      </c>
+      <c r="B42">
+        <v>12</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" t="s">
+        <v>47</v>
+      </c>
+      <c r="F42" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" t="s">
+        <v>38</v>
+      </c>
+      <c r="H42" t="s">
+        <v>37</v>
+      </c>
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>33</v>
+      </c>
+      <c r="B43">
+        <v>13</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D43" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" t="s">
+        <v>122</v>
+      </c>
+      <c r="F43" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" t="s">
+        <v>119</v>
+      </c>
+      <c r="H43" t="s">
+        <v>120</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>34</v>
+      </c>
+      <c r="B44">
+        <v>13</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" t="s">
+        <v>124</v>
+      </c>
+      <c r="F44" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" t="s">
+        <v>119</v>
+      </c>
+      <c r="H44" t="s">
+        <v>120</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>35</v>
+      </c>
+      <c r="B45">
+        <v>14</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D45" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" t="s">
+        <v>119</v>
+      </c>
+      <c r="H45" t="s">
+        <v>120</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>35</v>
+      </c>
+      <c r="B46">
+        <v>14</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D46" t="s">
+        <v>22</v>
+      </c>
+      <c r="F46" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" t="s">
+        <v>30</v>
+      </c>
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>37</v>
+      </c>
+      <c r="B47">
+        <v>14</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D47" t="s">
+        <v>78</v>
+      </c>
+      <c r="F47" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" t="s">
+        <v>26</v>
+      </c>
+      <c r="I47" s="1"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>37</v>
+      </c>
+      <c r="B48">
+        <v>14</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D48" t="s">
+        <v>44</v>
+      </c>
+      <c r="F48" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" t="s">
+        <v>32</v>
+      </c>
+      <c r="H48" t="s">
+        <v>43</v>
+      </c>
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>37</v>
+      </c>
+      <c r="B49">
+        <v>14</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D49" t="s">
+        <v>47</v>
+      </c>
+      <c r="F49" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" t="s">
+        <v>32</v>
+      </c>
+      <c r="H49" t="s">
+        <v>43</v>
+      </c>
+      <c r="I49" s="1"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C50" s="1"/>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="I50" s="1"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C51" s="1"/>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="I51" s="1"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C52" s="1"/>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="I52" s="1"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C53" s="1"/>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="I53" s="1"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C54" s="1"/>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="I54" s="1"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C55" s="1"/>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="I55" s="1"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C56" s="1"/>
-    </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="I56" s="1"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C57" s="1"/>
-    </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="I57" s="1"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C58" s="1"/>
-    </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="I58" s="1"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C59" s="1"/>
-    </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="I59" s="1"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C60" s="1"/>
-    </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="I60" s="1"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C61" s="1"/>
-    </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="I61" s="1"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C62" s="1"/>
-    </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="I62" s="1"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C63" s="1"/>
-    </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="I63" s="1"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C64" s="1"/>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="I64" s="1"/>
+    </row>
+    <row r="65" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C65" s="1"/>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="I65" s="1"/>
+    </row>
+    <row r="66" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C70" s="1"/>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C72" s="1"/>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C80" s="1"/>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.25">
@@ -1606,9 +2211,6 @@
     </row>
     <row r="104" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C104" s="1"/>
-    </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C105" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1618,10 +2220,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB70530A-5E05-4C30-BC42-1EFF983AD01B}">
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1881,6 +2483,120 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>7</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>10</v>
+      </c>
+      <c r="M6">
+        <v>8</v>
+      </c>
+      <c r="N6">
+        <v>9</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>31</v>
+      </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="P7">
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <v>4</v>
+      </c>
+      <c r="S7">
+        <v>3</v>
+      </c>
+      <c r="T7">
+        <v>5</v>
+      </c>
+      <c r="V7">
+        <v>8</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="Y7">
+        <v>7</v>
+      </c>
+      <c r="Z7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>7</v>
+      </c>
+      <c r="N8">
+        <v>8</v>
+      </c>
+      <c r="O8">
+        <v>6</v>
+      </c>
+      <c r="Y8">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update 23 24 dil
</commit_message>
<xml_diff>
--- a/survivor_2023_data.xlsx
+++ b/survivor_2023_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tina\Documents\GitHub\personal_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C13607-3272-4A3E-A89E-6ED4F55F3244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C52C80F-9C2A-495F-B796-DCB7A0F6FAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="3000" windowWidth="28545" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="event_log" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="191">
   <si>
     <t>DAY</t>
   </si>
@@ -586,6 +586,30 @@
   </si>
   <si>
     <t>1:12:14</t>
+  </si>
+  <si>
+    <t>Sloučení</t>
+  </si>
+  <si>
+    <t>11:28</t>
+  </si>
+  <si>
+    <t>Rivalové</t>
+  </si>
+  <si>
+    <t>Žaneta, Johanka, Kulhy, Adam, Martin, Barbora, Kristián, Pepa, Andrea, Karolína, Tomáš</t>
+  </si>
+  <si>
+    <t>13:48</t>
+  </si>
+  <si>
+    <t>Den 56</t>
+  </si>
+  <si>
+    <t>51:02</t>
+  </si>
+  <si>
+    <t>1:20:25</t>
   </si>
 </sst>
 </file>
@@ -939,11 +963,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I103"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2778,7 +2800,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B73">
         <v>22</v>
@@ -2802,7 +2824,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B74">
         <v>22</v>
@@ -2826,7 +2848,7 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B75">
         <v>22</v>
@@ -2849,19 +2871,93 @@
       <c r="I75" s="1"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C76" s="1"/>
+      <c r="A76">
+        <v>54</v>
+      </c>
+      <c r="B76">
+        <v>23</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D76" t="s">
+        <v>183</v>
+      </c>
+      <c r="F76" t="s">
+        <v>185</v>
+      </c>
+      <c r="G76" t="s">
+        <v>186</v>
+      </c>
       <c r="I76" s="1"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C77" s="1"/>
+      <c r="A77">
+        <v>56</v>
+      </c>
+      <c r="B77">
+        <v>24</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D77" t="s">
+        <v>22</v>
+      </c>
+      <c r="F77" t="s">
+        <v>185</v>
+      </c>
+      <c r="G77" t="s">
+        <v>24</v>
+      </c>
       <c r="I77" s="1"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C78" s="1"/>
+      <c r="A78">
+        <v>57</v>
+      </c>
+      <c r="B78">
+        <v>24</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D78" t="s">
+        <v>44</v>
+      </c>
+      <c r="F78" t="s">
+        <v>185</v>
+      </c>
+      <c r="G78" t="s">
+        <v>25</v>
+      </c>
+      <c r="H78" t="s">
+        <v>29</v>
+      </c>
       <c r="I78" s="1"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C79" s="1"/>
+      <c r="A79">
+        <v>57</v>
+      </c>
+      <c r="B79">
+        <v>24</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D79" t="s">
+        <v>47</v>
+      </c>
+      <c r="F79" t="s">
+        <v>185</v>
+      </c>
+      <c r="G79" t="s">
+        <v>29</v>
+      </c>
+      <c r="H79" t="s">
+        <v>25</v>
+      </c>
       <c r="I79" s="1"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -2910,7 +3006,6 @@
     </row>
     <row r="91" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C91" s="1"/>
-      <c r="I91" s="1"/>
     </row>
     <row r="92" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C92" s="1"/>
@@ -2944,9 +3039,6 @@
     </row>
     <row r="102" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C102" s="1"/>
-    </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C103" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2956,10 +3048,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB70530A-5E05-4C30-BC42-1EFF983AD01B}">
-  <dimension ref="A1:AA12"/>
+  <dimension ref="A1:AA13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3458,6 +3550,50 @@
         <v>3</v>
       </c>
     </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>188</v>
+      </c>
+      <c r="B13">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13">
+        <v>8</v>
+      </c>
+      <c r="L13">
+        <v>8</v>
+      </c>
+      <c r="N13">
+        <v>4</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
+      <c r="P13">
+        <v>4</v>
+      </c>
+      <c r="R13">
+        <v>8</v>
+      </c>
+      <c r="V13">
+        <v>8</v>
+      </c>
+      <c r="AA13">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
epizoda 30, pridanie hlasovani na kmenovych radach
</commit_message>
<xml_diff>
--- a/survivor_2023_data.xlsx
+++ b/survivor_2023_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tina\Documents\GitHub\personal_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04CFEA9-96AB-4638-BD92-F3AFD6D77279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E807970-DDF9-41FF-BFDC-60947D4B2A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="event_log" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="240">
   <si>
     <t>DAY</t>
   </si>
@@ -747,6 +747,18 @@
   </si>
   <si>
     <t>1:15:45</t>
+  </si>
+  <si>
+    <t>9:42</t>
+  </si>
+  <si>
+    <t>Den 71</t>
+  </si>
+  <si>
+    <t>47:58</t>
+  </si>
+  <si>
+    <t>1:12:00</t>
   </si>
 </sst>
 </file>
@@ -1107,10 +1119,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3631,6 +3643,90 @@
         <v>34</v>
       </c>
     </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>71</v>
+      </c>
+      <c r="B103">
+        <v>30</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D103" t="s">
+        <v>22</v>
+      </c>
+      <c r="F103" t="s">
+        <v>185</v>
+      </c>
+      <c r="G103" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>72</v>
+      </c>
+      <c r="B104">
+        <v>30</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D104" t="s">
+        <v>44</v>
+      </c>
+      <c r="F104" t="s">
+        <v>185</v>
+      </c>
+      <c r="G104" t="s">
+        <v>24</v>
+      </c>
+      <c r="H104" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>72</v>
+      </c>
+      <c r="B105">
+        <v>30</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D105" t="s">
+        <v>47</v>
+      </c>
+      <c r="F105" t="s">
+        <v>185</v>
+      </c>
+      <c r="G105" t="s">
+        <v>24</v>
+      </c>
+      <c r="H105" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C106" s="1"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C107" s="1"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C108" s="1"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C109" s="1"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C110" s="1"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C111" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3640,10 +3736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB70530A-5E05-4C30-BC42-1EFF983AD01B}">
-  <dimension ref="A1:AA18"/>
+  <dimension ref="A1:AA19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4358,6 +4454,32 @@
         <v>3</v>
       </c>
     </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>237</v>
+      </c>
+      <c r="B19">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="I19">
+        <v>4</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="L19">
+        <v>5</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4365,9 +4487,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CD196B6-7601-47F7-B845-102943A6C8E6}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4666,6 +4790,17 @@
       </c>
       <c r="C27">
         <v>0.1396</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>258000</v>
+      </c>
+      <c r="C28">
+        <v>0.12839999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -4675,12 +4810,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E86D9FE9-7F18-4BDA-98A7-6A3578215BD5}">
-  <dimension ref="A1:AA20"/>
+  <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5452,6 +5587,35 @@
         <v>30</v>
       </c>
     </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>225</v>
+      </c>
+      <c r="D21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
pridanie statistik skrytych imunit
</commit_message>
<xml_diff>
--- a/survivor_2023_data.xlsx
+++ b/survivor_2023_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tina\Documents\GitHub\personal_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E807970-DDF9-41FF-BFDC-60947D4B2A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836B57C2-4A29-4656-8652-664A3DA4FE3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="240">
   <si>
     <t>DAY</t>
   </si>
@@ -1121,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2652,6 +2652,9 @@
       <c r="G60" t="s">
         <v>36</v>
       </c>
+      <c r="H60" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
@@ -2978,6 +2981,9 @@
       <c r="G73" t="s">
         <v>29</v>
       </c>
+      <c r="H73" t="s">
+        <v>40</v>
+      </c>
       <c r="I73" s="1"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -3371,6 +3377,9 @@
       <c r="G90" t="s">
         <v>32</v>
       </c>
+      <c r="H90" t="s">
+        <v>32</v>
+      </c>
       <c r="I90" s="1"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -3595,6 +3604,9 @@
       </c>
       <c r="G100" t="s">
         <v>29</v>
+      </c>
+      <c r="H100" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -4810,18 +4822,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E86D9FE9-7F18-4BDA-98A7-6A3578215BD5}">
-  <dimension ref="A1:AA21"/>
+  <dimension ref="A1:AA22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
@@ -4835,22 +4847,22 @@
         <v>224</v>
       </c>
       <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>34</v>
-      </c>
-      <c r="G1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" t="s">
-        <v>24</v>
       </c>
       <c r="J1" t="s">
         <v>36</v>
@@ -4920,13 +4932,13 @@
       <c r="D2" t="s">
         <v>33</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>33</v>
       </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
       <c r="H2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" t="s">
         <v>33</v>
       </c>
       <c r="N2" t="s">
@@ -4958,11 +4970,11 @@
       <c r="C3" t="s">
         <v>225</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
         <v>39</v>
-      </c>
-      <c r="G3" t="s">
-        <v>35</v>
       </c>
       <c r="J3" t="s">
         <v>39</v>
@@ -5006,15 +5018,15 @@
         <v>225</v>
       </c>
       <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
         <v>29</v>
       </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
       <c r="H4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" t="s">
         <v>29</v>
       </c>
       <c r="K4" t="s">
@@ -5049,10 +5061,10 @@
       <c r="C5" t="s">
         <v>225</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" t="s">
         <v>37</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>37</v>
       </c>
       <c r="J5" t="s">
@@ -5068,7 +5080,7 @@
         <v>37</v>
       </c>
       <c r="R5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="S5" t="s">
         <v>37</v>
@@ -5093,14 +5105,14 @@
       <c r="D6" t="s">
         <v>33</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>52</v>
       </c>
       <c r="H6" t="s">
         <v>33</v>
-      </c>
-      <c r="I6" t="s">
-        <v>52</v>
       </c>
       <c r="K6" t="s">
         <v>26</v>
@@ -5132,15 +5144,15 @@
         <v>226</v>
       </c>
       <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
         <v>52</v>
       </c>
-      <c r="E7" t="s">
-        <v>33</v>
-      </c>
       <c r="H7" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" t="s">
         <v>52</v>
       </c>
       <c r="M7" t="s">
@@ -5166,14 +5178,14 @@
       <c r="C8" t="s">
         <v>225</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" t="s">
         <v>37</v>
-      </c>
-      <c r="G8" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" t="s">
-        <v>36</v>
       </c>
       <c r="J8" t="s">
         <v>40</v>
@@ -5204,11 +5216,11 @@
       <c r="C9" t="s">
         <v>226</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" t="s">
         <v>40</v>
-      </c>
-      <c r="I9" t="s">
-        <v>38</v>
       </c>
       <c r="J9" t="s">
         <v>40</v>
@@ -5237,10 +5249,10 @@
         <v>225</v>
       </c>
       <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
         <v>51</v>
-      </c>
-      <c r="E10" t="s">
-        <v>32</v>
       </c>
       <c r="H10" t="s">
         <v>51</v>
@@ -5271,11 +5283,11 @@
       <c r="C11" t="s">
         <v>225</v>
       </c>
-      <c r="F11" t="s">
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" t="s">
         <v>41</v>
-      </c>
-      <c r="G11" t="s">
-        <v>38</v>
       </c>
       <c r="I11" t="s">
         <v>41</v>
@@ -5290,7 +5302,7 @@
         <v>41</v>
       </c>
       <c r="Q11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R11" t="s">
         <v>41</v>
@@ -5306,25 +5318,25 @@
       <c r="C12" t="s">
         <v>225</v>
       </c>
-      <c r="F12" t="s">
+      <c r="E12" t="s">
         <v>36</v>
       </c>
       <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" t="s">
         <v>36</v>
-      </c>
-      <c r="I12" t="s">
-        <v>41</v>
       </c>
       <c r="J12" t="s">
         <v>34</v>
       </c>
+      <c r="O12" t="s">
+        <v>41</v>
+      </c>
       <c r="P12" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="Q12" t="s">
-        <v>36</v>
-      </c>
-      <c r="R12" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5338,7 +5350,7 @@
       <c r="C13" t="s">
         <v>225</v>
       </c>
-      <c r="F13" t="s">
+      <c r="E13" t="s">
         <v>36</v>
       </c>
       <c r="G13" t="s">
@@ -5367,14 +5379,14 @@
       <c r="C14" t="s">
         <v>225</v>
       </c>
-      <c r="F14" t="s">
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" t="s">
         <v>24</v>
-      </c>
-      <c r="G14" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" t="s">
-        <v>40</v>
       </c>
       <c r="J14" t="s">
         <v>40</v>
@@ -5393,10 +5405,10 @@
       <c r="C15" t="s">
         <v>226</v>
       </c>
-      <c r="F15" t="s">
+      <c r="E15" t="s">
         <v>28</v>
       </c>
-      <c r="G15" t="s">
+      <c r="I15" t="s">
         <v>28</v>
       </c>
     </row>
@@ -5414,10 +5426,10 @@
         <v>25</v>
       </c>
       <c r="E16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" t="s">
         <v>25</v>
-      </c>
-      <c r="F16" t="s">
-        <v>51</v>
       </c>
       <c r="G16" t="s">
         <v>51</v>
@@ -5458,10 +5470,10 @@
         <v>24</v>
       </c>
       <c r="E17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" t="s">
         <v>24</v>
-      </c>
-      <c r="F17" t="s">
-        <v>53</v>
       </c>
       <c r="G17" t="s">
         <v>53</v>
@@ -5499,10 +5511,10 @@
         <v>40</v>
       </c>
       <c r="E18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" t="s">
         <v>40</v>
-      </c>
-      <c r="F18" t="s">
-        <v>32</v>
       </c>
       <c r="G18" t="s">
         <v>32</v>
@@ -5537,10 +5549,10 @@
         <v>24</v>
       </c>
       <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" t="s">
         <v>24</v>
-      </c>
-      <c r="F19" t="s">
-        <v>32</v>
       </c>
       <c r="G19" t="s">
         <v>32</v>
@@ -5569,19 +5581,19 @@
         <v>225</v>
       </c>
       <c r="D20" t="s">
+        <v>227</v>
+      </c>
+      <c r="E20" t="s">
         <v>36</v>
       </c>
-      <c r="E20" t="s">
-        <v>227</v>
-      </c>
       <c r="F20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" t="s">
         <v>36</v>
       </c>
       <c r="H20" t="s">
         <v>36</v>
+      </c>
+      <c r="I20" t="s">
+        <v>30</v>
       </c>
       <c r="J20" t="s">
         <v>30</v>
@@ -5604,16 +5616,42 @@
         <v>24</v>
       </c>
       <c r="F21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" t="s">
         <v>32</v>
-      </c>
-      <c r="G21" t="s">
-        <v>24</v>
       </c>
       <c r="H21" t="s">
         <v>24</v>
       </c>
       <c r="I21" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <v>72</v>
+      </c>
+      <c r="C22" t="s">
+        <v>225</v>
+      </c>
+      <c r="D22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mensie opravy, opravy meta tagov
</commit_message>
<xml_diff>
--- a/survivor_2023_data.xlsx
+++ b/survivor_2023_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tina\Documents\GitHub\personal_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836B57C2-4A29-4656-8652-664A3DA4FE3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903792C2-83EC-4FD2-A974-82B1557161FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="event_log" sheetId="1" r:id="rId1"/>
@@ -1121,7 +1121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+    <sheetView topLeftCell="A79" workbookViewId="0">
       <selection activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
@@ -4499,10 +4499,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CD196B6-7601-47F7-B845-102943A6C8E6}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4813,6 +4813,17 @@
       </c>
       <c r="C28">
         <v>0.12839999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>292000</v>
+      </c>
+      <c r="C29">
+        <v>0.1525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>